<commit_message>
finalized project and provided a test spreadsheet for proof of concept
</commit_message>
<xml_diff>
--- a/vcards/Book1.xlsx
+++ b/vcards/Book1.xlsx
@@ -360,55 +360,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.42578125" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>